<commit_message>
test cases drafted -Cooper
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccnazar\PycharmProjects\cs151-lab7-harry_cooper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF27D802-FB15-694F-BF0B-8F3CB3EC9386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63128E43-A454-46AD-9714-F902803B4AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15855" windowHeight="11295" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>&lt;-- final overall cost</t>
   </si>
@@ -58,12 +58,24 @@
   </si>
   <si>
     <t>cost/sqft</t>
+  </si>
+  <si>
+    <t>Hardwood</t>
+  </si>
+  <si>
+    <t>Carpet</t>
+  </si>
+  <si>
+    <t>Tile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -205,18 +217,20 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
@@ -273,9 +287,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -313,7 +327,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -419,7 +433,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -561,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -572,35 +586,35 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -614,49 +628,106 @@
         <v>1</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1.39</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10">
+        <f>(B3*C3)*H2</f>
+        <v>695</v>
+      </c>
       <c r="E3" s="1"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="7">
+        <v>3.99</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="D4" s="10">
+        <f>(B4*C4)*H2</f>
+        <v>433.12399999999991</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4.99</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10">
+        <f>(B5*C5)*H3</f>
+        <v>1197</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>14.239000000000001</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="D6" s="10">
+        <f>(B6*C6)*H3</f>
+        <v>590.86154399999998</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>16.05</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10">
+        <f>(B7*C7)*H4</f>
+        <v>800.89499999999998</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>

</xml_diff>

<commit_message>
Total cost added to test cases -Cooper
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccnazar\PycharmProjects\cs151-lab7-harry_cooper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63128E43-A454-46AD-9714-F902803B4AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587E487-3205-4B5D-AA7F-F0E6A6F1CB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="15855" windowHeight="11295" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -226,11 +226,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
@@ -586,7 +586,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -600,13 +600,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
@@ -631,7 +631,7 @@
       <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>1.39</v>
       </c>
     </row>
@@ -645,7 +645,7 @@
       <c r="C3" s="3">
         <v>20</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <f>(B3*C3)*H2</f>
         <v>695</v>
       </c>
@@ -667,7 +667,7 @@
       <c r="C4" s="3">
         <v>15.2</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <f>(B4*C4)*H2</f>
         <v>433.12399999999991</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="C5" s="3">
         <v>15</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <f>(B5*C5)*H3</f>
         <v>1197</v>
       </c>
@@ -705,7 +705,7 @@
       <c r="C6" s="3">
         <v>10.4</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <f>(B6*C6)*H3</f>
         <v>590.86154399999998</v>
       </c>
@@ -721,7 +721,7 @@
       <c r="C7" s="3">
         <v>10</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <f>(B7*C7)*H4</f>
         <v>800.89499999999998</v>
       </c>
@@ -731,7 +731,10 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="9">
+        <f>D3+D4+D5+D6+D7</f>
+        <v>3716.8805439999996</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Test cases tested -Cooper
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccnazar\PycharmProjects\cs151-lab7-harry_cooper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587E487-3205-4B5D-AA7F-F0E6A6F1CB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701A83B4-499B-4681-BBCA-9412210C6E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="15855" windowHeight="11295" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>